<commit_message>
Added CPI. Added reading parameters for road maintenance.
</commit_message>
<xml_diff>
--- a/pycba/parameters/svk/transport/OPIIv3p0/svk_road_cba_parameters_OPIIv3p0_2022.xlsx
+++ b/pycba/parameters/svk/transport/OPIIv3p0/svk_road_cba_parameters_OPIIv3p0_2022.xlsx
@@ -5,11 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="residual_value" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="conversion_factors" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="operation_cost" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="cpi" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="cpi_meta" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="49">
   <si>
     <t xml:space="preserve">item</t>
   </si>
@@ -105,16 +108,81 @@
   </si>
   <si>
     <t xml:space="preserve">fuel_diesel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">surface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">condition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lower_usage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">price_level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">road</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tarmac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eur/m2/year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">concrete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">good</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bridge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tunnel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new_warranty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">guidebook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IFP_2022_03-59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -188,7 +256,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -206,6 +274,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -228,8 +308,8 @@
   </sheetPr>
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O39" activeCellId="0" sqref="O39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -391,7 +471,8 @@
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="3" t="b">
+      <c r="B11" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C11" s="2"/>
@@ -530,7 +611,7 @@
       <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -578,6 +659,732 @@
       </c>
       <c r="B6" s="1" t="n">
         <v>0.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.85"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="6" t="n">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="6" t="n">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="6" t="n">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="6" t="n">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="6" t="n">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="6" t="n">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="6" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="6" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="6" t="n">
+        <v>130.9</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="6" t="n">
+        <v>130.9</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="6" t="n">
+        <v>20.4</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="6" t="n">
+        <v>20.4</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="6" t="n">
+        <v>20.4</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="6" t="n">
+        <v>20.4</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>28.5</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.58"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B2" s="7" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C2" s="7" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.039</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0.039</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.036</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.014</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>-0.001</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>-0.003</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>-0.003</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>-0.005</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>-0.005</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0.025</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0.027</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0.027</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0.019</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0.032</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0.085</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.4"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added OPEX maintenance computation. Other.
</commit_message>
<xml_diff>
--- a/pycba/parameters/svk/transport/OPIIv3p0/svk_road_cba_parameters_OPIIv3p0_2022.xlsx
+++ b/pycba/parameters/svk/transport/OPIIv3p0/svk_road_cba_parameters_OPIIv3p0_2022.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="residual_value" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,8 @@
     <sheet name="operation_cost" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="cpi" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="cpi_meta" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="gdp_growth" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="gdp_growth_meta" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="50">
   <si>
     <t xml:space="preserve">item</t>
   </si>
@@ -108,6 +110,9 @@
   </si>
   <si>
     <t xml:space="preserve">fuel_diesel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">section_type</t>
   </si>
   <si>
     <t xml:space="preserve">surface</t>
@@ -256,36 +261,40 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -302,7 +311,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -601,7 +610,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -673,479 +682,498 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="13.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="13.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" s="5" t="s">
         <v>29</v>
       </c>
+      <c r="C1" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="E1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="F1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="B2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>2021</v>
-      </c>
-      <c r="F2" s="0" t="s">
+      <c r="C2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="6" t="n">
+      <c r="D2" s="6" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="7" t="n">
         <v>4.7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="6" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="G3" s="7" t="n">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>2021</v>
-      </c>
-      <c r="F3" s="0" t="s">
+      <c r="C4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="6" t="n">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="0" t="s">
+      <c r="D4" s="6" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="7" t="n">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="B5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="6" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="7" t="n">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="5" t="b">
+      <c r="C6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="7" t="n">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="6" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="E4" s="0" t="n">
-        <v>2021</v>
-      </c>
-      <c r="F4" s="0" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="6" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="5" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="7" t="n">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="6" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="5" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="6" t="n">
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="0" t="s">
+      <c r="D10" s="6" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="G10" s="7" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="6" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="5" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="7" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="5" t="b">
+      <c r="C12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="6" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="E5" s="0" t="n">
-        <v>2021</v>
-      </c>
-      <c r="F5" s="0" t="s">
+      <c r="E12" s="5" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="7" t="n">
+        <v>130.9</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="6" t="n">
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="0" t="s">
+      <c r="D13" s="6" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="7" t="n">
+        <v>130.9</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="6" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="7" t="n">
+        <v>20.4</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>2021</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="6" t="n">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="0" t="s">
+      <c r="C15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="6" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="G15" s="7" t="n">
+        <v>20.4</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="6" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="5" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="7" t="n">
+        <v>20.4</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>2021</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="0" t="s">
+      <c r="C17" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="6" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="7" t="n">
+        <v>20.4</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="6" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="5" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="5" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="6" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="5" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G19" s="5" t="n">
+        <v>28.5</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>2021</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="6" t="n">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="0" t="s">
+      <c r="D20" s="6" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="5" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>2021</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <v>2021</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="6" t="n">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <v>2021</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="6" t="n">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>2021</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="6" t="n">
-        <v>130.9</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <v>2021</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" s="6" t="n">
-        <v>130.9</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <v>2021</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" s="6" t="n">
-        <v>20.4</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E15" s="0" t="n">
-        <v>2021</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" s="6" t="n">
-        <v>20.4</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E16" s="0" t="n">
-        <v>2021</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G16" s="6" t="n">
-        <v>20.4</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E17" s="0" t="n">
-        <v>2021</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G17" s="6" t="n">
-        <v>20.4</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E18" s="0" t="n">
-        <v>2021</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G18" s="0" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E19" s="0" t="n">
-        <v>2021</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G19" s="0" t="n">
-        <v>28.5</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E20" s="0" t="n">
-        <v>2021</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G20" s="0" t="n">
+      <c r="G20" s="5" t="n">
         <v>35</v>
       </c>
     </row>
@@ -1161,169 +1189,169 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="14.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" s="5" t="s">
         <v>45</v>
       </c>
+      <c r="C1" s="5" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="5" t="n">
         <v>2010</v>
       </c>
-      <c r="B2" s="7" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="C2" s="7" t="n">
+      <c r="B2" s="8" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C2" s="8" t="n">
         <v>0.01</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="5" t="n">
         <v>2011</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="5" t="n">
         <v>0.039</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="5" t="n">
         <v>0.039</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="5" t="n">
         <v>2012</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="5" t="n">
         <v>0.036</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="5" t="n">
         <v>0.036</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="5" t="n">
         <v>2013</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="5" t="n">
         <v>0.014</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="5" t="n">
         <v>0.014</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="5" t="n">
         <v>2014</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="5" t="n">
         <v>-0.001</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="5" t="n">
         <v>-0.001</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="5" t="n">
         <v>2015</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="5" t="n">
         <v>-0.003</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="5" t="n">
         <v>-0.003</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="5" t="n">
         <v>2016</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="5" t="n">
         <v>-0.005</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="5" t="n">
         <v>-0.005</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="5" t="n">
         <v>2017</v>
       </c>
-      <c r="B9" s="0" t="n">
-        <v>0.013</v>
-      </c>
-      <c r="C9" s="0" t="n">
+      <c r="B9" s="5" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="C9" s="5" t="n">
         <v>0.013</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="5" t="n">
         <v>2018</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="5" t="n">
         <v>0.025</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="5" t="n">
         <v>0.025</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="5" t="n">
         <v>2019</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="5" t="n">
         <v>0.027</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="5" t="n">
         <v>0.027</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="5" t="n">
         <v>2020</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="5" t="n">
         <v>0.019</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="5" t="n">
         <v>0.019</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>2021</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <v>0.012</v>
-      </c>
-      <c r="C13" s="0" t="n">
+      <c r="A13" s="5" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B13" s="5" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="C13" s="5" t="n">
         <v>0.032</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="5" t="n">
         <v>2022</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="5" t="n">
         <v>0.085</v>
       </c>
     </row>
@@ -1339,52 +1367,598 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="16.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="16.39"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C42"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B2" s="5" t="n">
+        <v>-0.058</v>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>-0.044</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>0.039</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>0.021</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>0.053</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>0.018</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="n">
+        <v>2025</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>0.018</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="n">
+        <v>2026</v>
+      </c>
+      <c r="B8" s="5" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>0.017</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="n">
+        <v>2027</v>
+      </c>
+      <c r="B9" s="5" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>0.017</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="n">
+        <v>2028</v>
+      </c>
+      <c r="B10" s="5" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="C10" s="5" t="n">
+        <v>0.017</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="n">
+        <v>2029</v>
+      </c>
+      <c r="B11" s="5" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="C11" s="5" t="n">
+        <v>0.017</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="n">
+        <v>2030</v>
+      </c>
+      <c r="B12" s="5" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="C12" s="5" t="n">
+        <v>0.012</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="n">
+        <v>2031</v>
+      </c>
+      <c r="B13" s="5" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="C13" s="5" t="n">
+        <v>0.012</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="n">
+        <v>2032</v>
+      </c>
+      <c r="B14" s="5" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="C14" s="5" t="n">
+        <v>0.012</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="n">
+        <v>2033</v>
+      </c>
+      <c r="B15" s="5" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="C15" s="5" t="n">
+        <v>0.012</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="n">
+        <v>2034</v>
+      </c>
+      <c r="B16" s="5" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="C16" s="5" t="n">
+        <v>0.012</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="n">
+        <v>2035</v>
+      </c>
+      <c r="B17" s="5" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="C17" s="5" t="n">
+        <v>0.012</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="n">
+        <v>2036</v>
+      </c>
+      <c r="B18" s="5" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="C18" s="5" t="n">
+        <v>0.012</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="n">
+        <v>2037</v>
+      </c>
+      <c r="B19" s="5" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="C19" s="5" t="n">
+        <v>0.012</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="n">
+        <v>2038</v>
+      </c>
+      <c r="B20" s="5" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="C20" s="5" t="n">
+        <v>0.012</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="n">
+        <v>2039</v>
+      </c>
+      <c r="B21" s="5" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="C21" s="5" t="n">
+        <v>0.012</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="n">
+        <v>2040</v>
+      </c>
+      <c r="B22" s="5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C22" s="5" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="n">
+        <v>2041</v>
+      </c>
+      <c r="B23" s="5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C23" s="5" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="n">
+        <v>2042</v>
+      </c>
+      <c r="B24" s="5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C24" s="5" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5" t="n">
+        <v>2043</v>
+      </c>
+      <c r="B25" s="5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C25" s="5" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="n">
+        <v>2044</v>
+      </c>
+      <c r="B26" s="5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C26" s="5" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="n">
+        <v>2045</v>
+      </c>
+      <c r="B27" s="5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C27" s="5" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="n">
+        <v>2046</v>
+      </c>
+      <c r="B28" s="5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C28" s="5" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5" t="n">
+        <v>2047</v>
+      </c>
+      <c r="B29" s="5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C29" s="5" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5" t="n">
+        <v>2048</v>
+      </c>
+      <c r="B30" s="5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C30" s="5" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="n">
+        <v>2049</v>
+      </c>
+      <c r="B31" s="5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C31" s="5" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="n">
+        <v>2050</v>
+      </c>
+      <c r="B32" s="5" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="C32" s="5" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="5" t="n">
+        <v>2051</v>
+      </c>
+      <c r="B33" s="5" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="C33" s="5" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="5" t="n">
+        <v>2052</v>
+      </c>
+      <c r="B34" s="5" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="C34" s="5" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="5" t="n">
+        <v>2053</v>
+      </c>
+      <c r="B35" s="5" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="C35" s="5" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="5" t="n">
+        <v>2054</v>
+      </c>
+      <c r="B36" s="5" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="C36" s="5" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="5" t="n">
+        <v>2055</v>
+      </c>
+      <c r="B37" s="5" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="C37" s="5" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="5" t="n">
+        <v>2056</v>
+      </c>
+      <c r="B38" s="5" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="C38" s="5" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="5" t="n">
+        <v>2057</v>
+      </c>
+      <c r="B39" s="5" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="C39" s="5" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="5" t="n">
+        <v>2058</v>
+      </c>
+      <c r="B40" s="5" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="C40" s="5" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="5" t="n">
+        <v>2059</v>
+      </c>
+      <c r="B41" s="5" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="C41" s="5" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="5" t="n">
+        <v>2060</v>
+      </c>
+      <c r="B42" s="5" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="C42" s="5" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="14.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="15.18"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
         <v>47</v>
       </c>
+      <c r="B1" s="5" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>44</v>
+      <c r="B3" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>45</v>
+      <c r="A4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Compute fuel cost saving.
</commit_message>
<xml_diff>
--- a/pycba/parameters/svk/transport/OPIIv3p0/svk_road_cba_parameters_OPIIv3p0_2022.xlsx
+++ b/pycba/parameters/svk/transport/OPIIv3p0/svk_road_cba_parameters_OPIIv3p0_2022.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="residual_value" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,14 +13,18 @@
     <sheet name="operation_cost" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="vtts" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="passenger_occupancy" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="trip_purpose" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="voc_l" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="voc_l" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="trip_purpose" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="voc_t" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="fuel_ratio" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="cpi" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="cpi_meta" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="gdp_growth" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="gdp_growth_meta" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="fuel_consumption" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="fuel_density" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="fuel_cost" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="fuel_consumption_acceleration" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="cpi" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="cpi_meta" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="gdp_growth" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="gdp_growth_meta" sheetId="17" state="visible" r:id="rId18"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -32,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="83">
   <si>
     <t xml:space="preserve">item</t>
   </si>
@@ -196,34 +200,73 @@
     <t xml:space="preserve">bus</t>
   </si>
   <si>
+    <t xml:space="preserve">fuel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">petrol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eur/veh/km</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diesel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lgv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mgv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hgv</t>
+  </si>
+  <si>
     <t xml:space="preserve">transit</t>
   </si>
   <si>
     <t xml:space="preserve">train</t>
   </si>
   <si>
-    <t xml:space="preserve">fuel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">petrol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eur/veh/km</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diesel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lgv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mgv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hgv</t>
-  </si>
-  <si>
     <t xml:space="preserve">eur/veh/h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l/km</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kg/l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eur/l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exit_intravilan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">roundabout_intravilan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">roundabout_extravilan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intersection_intravilan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intersection_extravilan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interchange</t>
   </si>
   <si>
     <t xml:space="preserve">year</t>
@@ -248,12 +291,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.00E+00"/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -327,7 +371,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -364,6 +408,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,7 +432,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O39" activeCellId="1" sqref="E10:E11 O39"/>
+      <selection pane="topLeft" activeCell="O39" activeCellId="0" sqref="O39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -680,166 +728,173 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="E10:E11 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="14.58"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>66</v>
       </c>
+      <c r="G1" s="5" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="n">
-        <v>2010</v>
-      </c>
-      <c r="B2" s="8" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="C2" s="8" t="n">
-        <v>0.01</v>
+      <c r="A2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>0.143</v>
+      </c>
+      <c r="E2" s="8" t="n">
+        <v>-0.00234</v>
+      </c>
+      <c r="F2" s="8" t="n">
+        <v>1.61E-005</v>
+      </c>
+      <c r="G2" s="8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="n">
-        <v>2011</v>
-      </c>
-      <c r="B3" s="5" t="n">
-        <v>0.039</v>
-      </c>
-      <c r="C3" s="5" t="n">
-        <v>0.039</v>
+      <c r="A3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>0.133</v>
+      </c>
+      <c r="E3" s="8" t="n">
+        <v>-0.00234</v>
+      </c>
+      <c r="F3" s="8" t="n">
+        <v>1.61E-005</v>
+      </c>
+      <c r="G3" s="8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="n">
-        <v>2012</v>
-      </c>
-      <c r="B4" s="5" t="n">
-        <v>0.036</v>
-      </c>
-      <c r="C4" s="5" t="n">
-        <v>0.036</v>
+      <c r="A4" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>0.173</v>
+      </c>
+      <c r="E4" s="8" t="n">
+        <v>-0.00234</v>
+      </c>
+      <c r="F4" s="8" t="n">
+        <v>1.61E-005</v>
+      </c>
+      <c r="G4" s="8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="n">
-        <v>2013</v>
-      </c>
-      <c r="B5" s="5" t="n">
-        <v>0.014</v>
-      </c>
-      <c r="C5" s="5" t="n">
-        <v>0.014</v>
+      <c r="A5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>0.883</v>
+      </c>
+      <c r="E5" s="8" t="n">
+        <v>-0.0217</v>
+      </c>
+      <c r="F5" s="8" t="n">
+        <v>0.000262</v>
+      </c>
+      <c r="G5" s="8" t="n">
+        <v>-9.89E-007</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="n">
-        <v>2014</v>
-      </c>
-      <c r="B6" s="5" t="n">
-        <v>-0.001</v>
-      </c>
-      <c r="C6" s="5" t="n">
-        <v>-0.001</v>
+      <c r="A6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>1.024</v>
+      </c>
+      <c r="E6" s="8" t="n">
+        <v>-0.0217</v>
+      </c>
+      <c r="F6" s="8" t="n">
+        <v>0.000262</v>
+      </c>
+      <c r="G6" s="8" t="n">
+        <v>-9.89E-007</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="n">
-        <v>2015</v>
-      </c>
-      <c r="B7" s="5" t="n">
-        <v>-0.003</v>
-      </c>
-      <c r="C7" s="5" t="n">
-        <v>-0.003</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="n">
-        <v>2016</v>
-      </c>
-      <c r="B8" s="5" t="n">
-        <v>-0.005</v>
-      </c>
-      <c r="C8" s="5" t="n">
-        <v>-0.005</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="n">
-        <v>2017</v>
-      </c>
-      <c r="B9" s="5" t="n">
-        <v>0.013</v>
-      </c>
-      <c r="C9" s="5" t="n">
-        <v>0.013</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="n">
-        <v>2018</v>
-      </c>
-      <c r="B10" s="5" t="n">
-        <v>0.025</v>
-      </c>
-      <c r="C10" s="5" t="n">
-        <v>0.025</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="n">
-        <v>2019</v>
-      </c>
-      <c r="B11" s="5" t="n">
-        <v>0.027</v>
-      </c>
-      <c r="C11" s="5" t="n">
-        <v>0.027</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="n">
-        <v>2020</v>
-      </c>
-      <c r="B12" s="5" t="n">
-        <v>0.019</v>
-      </c>
-      <c r="C12" s="5" t="n">
-        <v>0.019</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="n">
-        <v>2021</v>
-      </c>
-      <c r="B13" s="5" t="n">
-        <v>0.012</v>
-      </c>
-      <c r="C13" s="5" t="n">
-        <v>0.032</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="n">
-        <v>2022</v>
-      </c>
-      <c r="C14" s="5" t="n">
-        <v>0.085</v>
+      <c r="A7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>0.703</v>
+      </c>
+      <c r="E7" s="8" t="n">
+        <v>-0.0217</v>
+      </c>
+      <c r="F7" s="8" t="n">
+        <v>0.000262</v>
+      </c>
+      <c r="G7" s="8" t="n">
+        <v>-9.89E-007</v>
       </c>
     </row>
   </sheetData>
@@ -858,48 +913,45 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="E10:E11 B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="16.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="16.39"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>68</v>
+        <v>33</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>66</v>
+      <c r="C2" s="5" t="n">
+        <v>0.72</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>66</v>
+        <v>69</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>0.82</v>
       </c>
     </row>
   </sheetData>
@@ -918,474 +970,57 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="1" sqref="E10:E11 D7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="9.29"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>66</v>
+        <v>24</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="n">
-        <v>2020</v>
-      </c>
-      <c r="B2" s="5" t="n">
-        <v>-0.058</v>
+      <c r="A2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="C2" s="5" t="n">
-        <v>-0.044</v>
+        <v>0.523</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>2021</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="n">
-        <v>2021</v>
-      </c>
-      <c r="B3" s="5" t="n">
-        <v>0.043</v>
-      </c>
-      <c r="C3" s="5" t="n">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="n">
-        <v>2022</v>
-      </c>
-      <c r="B4" s="5" t="n">
-        <v>0.039</v>
-      </c>
-      <c r="C4" s="5" t="n">
-        <v>0.021</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="n">
-        <v>2023</v>
-      </c>
-      <c r="B5" s="5" t="n">
-        <v>0.025</v>
-      </c>
-      <c r="C5" s="5" t="n">
-        <v>0.053</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="n">
-        <v>2024</v>
-      </c>
-      <c r="B6" s="5" t="n">
-        <v>0.007</v>
-      </c>
-      <c r="C6" s="5" t="n">
-        <v>0.018</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="B7" s="5" t="n">
-        <v>0.017</v>
-      </c>
-      <c r="C7" s="5" t="n">
-        <v>0.018</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B8" s="5" t="n">
-        <v>0.017</v>
-      </c>
-      <c r="C8" s="5" t="n">
-        <v>0.017</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="n">
-        <v>2027</v>
-      </c>
-      <c r="B9" s="5" t="n">
-        <v>0.017</v>
-      </c>
-      <c r="C9" s="5" t="n">
-        <v>0.017</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="n">
-        <v>2028</v>
-      </c>
-      <c r="B10" s="5" t="n">
-        <v>0.017</v>
-      </c>
-      <c r="C10" s="5" t="n">
-        <v>0.017</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="n">
-        <v>2029</v>
-      </c>
-      <c r="B11" s="5" t="n">
-        <v>0.017</v>
-      </c>
-      <c r="C11" s="5" t="n">
-        <v>0.017</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="n">
-        <v>2030</v>
-      </c>
-      <c r="B12" s="5" t="n">
-        <v>0.012</v>
-      </c>
-      <c r="C12" s="5" t="n">
-        <v>0.012</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="n">
-        <v>2031</v>
-      </c>
-      <c r="B13" s="5" t="n">
-        <v>0.012</v>
-      </c>
-      <c r="C13" s="5" t="n">
-        <v>0.012</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="n">
-        <v>2032</v>
-      </c>
-      <c r="B14" s="5" t="n">
-        <v>0.012</v>
-      </c>
-      <c r="C14" s="5" t="n">
-        <v>0.012</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="n">
-        <v>2033</v>
-      </c>
-      <c r="B15" s="5" t="n">
-        <v>0.012</v>
-      </c>
-      <c r="C15" s="5" t="n">
-        <v>0.012</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="n">
-        <v>2034</v>
-      </c>
-      <c r="B16" s="5" t="n">
-        <v>0.012</v>
-      </c>
-      <c r="C16" s="5" t="n">
-        <v>0.012</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="n">
-        <v>2035</v>
-      </c>
-      <c r="B17" s="5" t="n">
-        <v>0.012</v>
-      </c>
-      <c r="C17" s="5" t="n">
-        <v>0.012</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="n">
-        <v>2036</v>
-      </c>
-      <c r="B18" s="5" t="n">
-        <v>0.012</v>
-      </c>
-      <c r="C18" s="5" t="n">
-        <v>0.012</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="n">
-        <v>2037</v>
-      </c>
-      <c r="B19" s="5" t="n">
-        <v>0.012</v>
-      </c>
-      <c r="C19" s="5" t="n">
-        <v>0.012</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="n">
-        <v>2038</v>
-      </c>
-      <c r="B20" s="5" t="n">
-        <v>0.012</v>
-      </c>
-      <c r="C20" s="5" t="n">
-        <v>0.012</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="n">
-        <v>2039</v>
-      </c>
-      <c r="B21" s="5" t="n">
-        <v>0.012</v>
-      </c>
-      <c r="C21" s="5" t="n">
-        <v>0.012</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="n">
-        <v>2040</v>
-      </c>
-      <c r="B22" s="5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="C22" s="5" t="n">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="n">
-        <v>2041</v>
-      </c>
-      <c r="B23" s="5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="C23" s="5" t="n">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="n">
-        <v>2042</v>
-      </c>
-      <c r="B24" s="5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="C24" s="5" t="n">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="n">
-        <v>2043</v>
-      </c>
-      <c r="B25" s="5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="C25" s="5" t="n">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="n">
-        <v>2044</v>
-      </c>
-      <c r="B26" s="5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="C26" s="5" t="n">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="n">
-        <v>2045</v>
-      </c>
-      <c r="B27" s="5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="C27" s="5" t="n">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="n">
-        <v>2046</v>
-      </c>
-      <c r="B28" s="5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="C28" s="5" t="n">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="n">
-        <v>2047</v>
-      </c>
-      <c r="B29" s="5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="C29" s="5" t="n">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5" t="n">
-        <v>2048</v>
-      </c>
-      <c r="B30" s="5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="C30" s="5" t="n">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="n">
-        <v>2049</v>
-      </c>
-      <c r="B31" s="5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="C31" s="5" t="n">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="n">
-        <v>2050</v>
-      </c>
-      <c r="B32" s="5" t="n">
-        <v>0.013</v>
-      </c>
-      <c r="C32" s="5" t="n">
-        <v>0.013</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="n">
-        <v>2051</v>
-      </c>
-      <c r="B33" s="5" t="n">
-        <v>0.013</v>
-      </c>
-      <c r="C33" s="5" t="n">
-        <v>0.013</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5" t="n">
-        <v>2052</v>
-      </c>
-      <c r="B34" s="5" t="n">
-        <v>0.013</v>
-      </c>
-      <c r="C34" s="5" t="n">
-        <v>0.013</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="n">
-        <v>2053</v>
-      </c>
-      <c r="B35" s="5" t="n">
-        <v>0.013</v>
-      </c>
-      <c r="C35" s="5" t="n">
-        <v>0.013</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="n">
-        <v>2054</v>
-      </c>
-      <c r="B36" s="5" t="n">
-        <v>0.013</v>
-      </c>
-      <c r="C36" s="5" t="n">
-        <v>0.013</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5" t="n">
-        <v>2055</v>
-      </c>
-      <c r="B37" s="5" t="n">
-        <v>0.013</v>
-      </c>
-      <c r="C37" s="5" t="n">
-        <v>0.013</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="n">
-        <v>2056</v>
-      </c>
-      <c r="B38" s="5" t="n">
-        <v>0.013</v>
-      </c>
-      <c r="C38" s="5" t="n">
-        <v>0.013</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="5" t="n">
-        <v>2057</v>
-      </c>
-      <c r="B39" s="5" t="n">
-        <v>0.013</v>
-      </c>
-      <c r="C39" s="5" t="n">
-        <v>0.013</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5" t="n">
-        <v>2058</v>
-      </c>
-      <c r="B40" s="5" t="n">
-        <v>0.013</v>
-      </c>
-      <c r="C40" s="5" t="n">
-        <v>0.013</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="n">
-        <v>2059</v>
-      </c>
-      <c r="B41" s="5" t="n">
-        <v>0.013</v>
-      </c>
-      <c r="C41" s="5" t="n">
-        <v>0.013</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5" t="n">
-        <v>2060</v>
-      </c>
-      <c r="B42" s="5" t="n">
-        <v>0.013</v>
-      </c>
-      <c r="C42" s="5" t="n">
-        <v>0.013</v>
+      <c r="A3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="9" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>2021</v>
       </c>
     </row>
   </sheetData>
@@ -1404,10 +1039,943 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="12.61"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>0.057</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>0.024</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>0.081</v>
+      </c>
+      <c r="F2" s="5" t="n">
+        <v>0.033</v>
+      </c>
+      <c r="G2" s="5" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="H2" s="5" t="n">
+        <v>0.115</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>0.051</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>0.073</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="G3" s="5" t="n">
+        <v>0.081</v>
+      </c>
+      <c r="H3" s="5" t="n">
+        <v>0.103</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>0.029</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>0.099</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="H4" s="5" t="n">
+        <v>0.141</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>0.276</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>0.131</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>0.407</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>0.184</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="H5" s="5" t="n">
+        <v>0.519</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>0.393</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>0.165</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>0.558</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>0.228</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>0.621</v>
+      </c>
+      <c r="H6" s="5" t="n">
+        <v>0.804</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>0.256</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>0.123</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>0.379</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>0.174</v>
+      </c>
+      <c r="G7" s="5" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="H7" s="5" t="n">
+        <v>0.477</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="14.58"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B2" s="9" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C2" s="9" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>0.039</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>0.039</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>0.036</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>0.014</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>-0.001</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>-0.003</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>-0.003</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B8" s="5" t="n">
+        <v>-0.005</v>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>-0.005</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B9" s="5" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B10" s="5" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="C10" s="5" t="n">
+        <v>0.025</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B11" s="5" t="n">
+        <v>0.027</v>
+      </c>
+      <c r="C11" s="5" t="n">
+        <v>0.027</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B12" s="5" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="C12" s="5" t="n">
+        <v>0.019</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B13" s="5" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="C13" s="5" t="n">
+        <v>0.032</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C14" s="5" t="n">
+        <v>0.085</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="1" sqref="E10:E11 B9"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="16.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="16.39"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C42"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B2" s="5" t="n">
+        <v>-0.058</v>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>-0.044</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>0.039</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>0.021</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>0.053</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>0.018</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="n">
+        <v>2025</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>0.018</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="n">
+        <v>2026</v>
+      </c>
+      <c r="B8" s="5" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>0.017</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="n">
+        <v>2027</v>
+      </c>
+      <c r="B9" s="5" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>0.017</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="n">
+        <v>2028</v>
+      </c>
+      <c r="B10" s="5" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="C10" s="5" t="n">
+        <v>0.017</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="n">
+        <v>2029</v>
+      </c>
+      <c r="B11" s="5" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="C11" s="5" t="n">
+        <v>0.017</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="n">
+        <v>2030</v>
+      </c>
+      <c r="B12" s="5" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="C12" s="5" t="n">
+        <v>0.012</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="n">
+        <v>2031</v>
+      </c>
+      <c r="B13" s="5" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="C13" s="5" t="n">
+        <v>0.012</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="n">
+        <v>2032</v>
+      </c>
+      <c r="B14" s="5" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="C14" s="5" t="n">
+        <v>0.012</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="n">
+        <v>2033</v>
+      </c>
+      <c r="B15" s="5" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="C15" s="5" t="n">
+        <v>0.012</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="n">
+        <v>2034</v>
+      </c>
+      <c r="B16" s="5" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="C16" s="5" t="n">
+        <v>0.012</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="n">
+        <v>2035</v>
+      </c>
+      <c r="B17" s="5" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="C17" s="5" t="n">
+        <v>0.012</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="n">
+        <v>2036</v>
+      </c>
+      <c r="B18" s="5" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="C18" s="5" t="n">
+        <v>0.012</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="n">
+        <v>2037</v>
+      </c>
+      <c r="B19" s="5" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="C19" s="5" t="n">
+        <v>0.012</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="n">
+        <v>2038</v>
+      </c>
+      <c r="B20" s="5" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="C20" s="5" t="n">
+        <v>0.012</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="n">
+        <v>2039</v>
+      </c>
+      <c r="B21" s="5" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="C21" s="5" t="n">
+        <v>0.012</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="n">
+        <v>2040</v>
+      </c>
+      <c r="B22" s="5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C22" s="5" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="n">
+        <v>2041</v>
+      </c>
+      <c r="B23" s="5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C23" s="5" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="n">
+        <v>2042</v>
+      </c>
+      <c r="B24" s="5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C24" s="5" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5" t="n">
+        <v>2043</v>
+      </c>
+      <c r="B25" s="5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C25" s="5" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="n">
+        <v>2044</v>
+      </c>
+      <c r="B26" s="5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C26" s="5" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="n">
+        <v>2045</v>
+      </c>
+      <c r="B27" s="5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C27" s="5" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="n">
+        <v>2046</v>
+      </c>
+      <c r="B28" s="5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C28" s="5" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5" t="n">
+        <v>2047</v>
+      </c>
+      <c r="B29" s="5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C29" s="5" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5" t="n">
+        <v>2048</v>
+      </c>
+      <c r="B30" s="5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C30" s="5" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="n">
+        <v>2049</v>
+      </c>
+      <c r="B31" s="5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C31" s="5" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="n">
+        <v>2050</v>
+      </c>
+      <c r="B32" s="5" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="C32" s="5" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="5" t="n">
+        <v>2051</v>
+      </c>
+      <c r="B33" s="5" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="C33" s="5" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="5" t="n">
+        <v>2052</v>
+      </c>
+      <c r="B34" s="5" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="C34" s="5" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="5" t="n">
+        <v>2053</v>
+      </c>
+      <c r="B35" s="5" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="C35" s="5" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="5" t="n">
+        <v>2054</v>
+      </c>
+      <c r="B36" s="5" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="C36" s="5" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="5" t="n">
+        <v>2055</v>
+      </c>
+      <c r="B37" s="5" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="C37" s="5" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="5" t="n">
+        <v>2056</v>
+      </c>
+      <c r="B38" s="5" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="C38" s="5" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="5" t="n">
+        <v>2057</v>
+      </c>
+      <c r="B39" s="5" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="C39" s="5" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="5" t="n">
+        <v>2058</v>
+      </c>
+      <c r="B40" s="5" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="C40" s="5" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="5" t="n">
+        <v>2059</v>
+      </c>
+      <c r="B41" s="5" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="C41" s="5" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="5" t="n">
+        <v>2060</v>
+      </c>
+      <c r="B42" s="5" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="C42" s="5" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1418,34 +1986,34 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1467,7 +2035,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J15" activeCellId="1" sqref="E10:E11 J15"/>
+      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1539,7 +2107,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="E10:E11 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2046,7 +2614,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="1" sqref="E10:E11 E5"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2138,7 +2706,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H18" activeCellId="1" sqref="E10:E11 H18"/>
+      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2192,10 +2760,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="E10:E11 B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2205,69 +2773,118 @@
         <v>50</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>49</v>
+        <v>24</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="5" t="n">
-        <v>0.073</v>
-      </c>
-      <c r="C2" s="5" t="n">
-        <v>0.244</v>
+      <c r="B2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="D2" s="5" t="n">
-        <v>0.683</v>
+        <v>0.041</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>2021</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="5" t="n">
-        <v>0.037</v>
-      </c>
-      <c r="C3" s="5" t="n">
-        <v>0.338</v>
+        <v>51</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>0.625</v>
+        <v>0.034</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>2021</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="5" t="n">
-        <v>0.038</v>
-      </c>
-      <c r="C4" s="5" t="n">
-        <v>0.392</v>
+        <v>58</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>0.57</v>
+        <v>0.042</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>2021</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="5" t="n">
-        <v>0.043</v>
-      </c>
-      <c r="C5" s="5" t="n">
-        <v>0.256</v>
+        <v>59</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>0.701</v>
+        <v>0.065</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>0.084</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>2021</v>
       </c>
     </row>
   </sheetData>
@@ -2286,10 +2903,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="1" sqref="E10:E11 E7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2299,118 +2916,69 @@
         <v>50</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>58</v>
+      <c r="B2" s="5" t="n">
+        <v>0.073</v>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>0.244</v>
       </c>
       <c r="D2" s="5" t="n">
-        <v>0.041</v>
-      </c>
-      <c r="E2" s="5" t="n">
-        <v>2021</v>
+        <v>0.683</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>0.037</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>0.338</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>0.034</v>
-      </c>
-      <c r="E3" s="5" t="n">
-        <v>2021</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>0.038</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>0.392</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>0.042</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <v>2021</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>58</v>
+        <v>62</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>0.256</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>0.065</v>
-      </c>
-      <c r="E5" s="5" t="n">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="5" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="E6" s="5" t="n">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="5" t="n">
-        <v>0.084</v>
-      </c>
-      <c r="E7" s="5" t="n">
-        <v>2021</v>
+        <v>0.701</v>
       </c>
     </row>
   </sheetData>
@@ -2432,7 +3000,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="1" sqref="E10:E11 D8"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2442,7 +3010,7 @@
         <v>50</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>33</v>
@@ -2459,7 +3027,7 @@
         <v>51</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>63</v>
@@ -2476,7 +3044,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>63</v>
@@ -2490,10 +3058,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>63</v>
@@ -2507,10 +3075,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>63</v>
@@ -2524,10 +3092,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>63</v>
@@ -2544,7 +3112,7 @@
         <v>53</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>63</v>
@@ -2574,86 +3142,86 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10:E11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="5" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="B5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="0" t="n">
+      <c r="B6" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="5" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="0" t="n">
+      <c r="B7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="5" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Compute greenhouse gases' external costs.
</commit_message>
<xml_diff>
--- a/pycba/parameters/svk/transport/OPIIv3p0/svk_road_cba_parameters_OPIIv3p0_2022.xlsx
+++ b/pycba/parameters/svk/transport/OPIIv3p0/svk_road_cba_parameters_OPIIv3p0_2022.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="residual_value" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,6 +25,8 @@
     <sheet name="cpi_meta" sheetId="15" state="visible" r:id="rId16"/>
     <sheet name="gdp_growth" sheetId="16" state="visible" r:id="rId17"/>
     <sheet name="gdp_growth_meta" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="co2_cost" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="greenhouse_rate" sheetId="19" state="visible" r:id="rId20"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="91">
   <si>
     <t xml:space="preserve">item</t>
   </si>
@@ -285,6 +287,30 @@
   </si>
   <si>
     <t xml:space="preserve">newest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eur/tco2e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">co2e_factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">co2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g/kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ch4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n2o</t>
   </si>
 </sst>
 </file>
@@ -730,7 +756,7 @@
   </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -915,7 +941,7 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -972,7 +998,7 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -991,7 +1017,7 @@
       <c r="C1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1005,7 +1031,7 @@
       <c r="C2" s="5" t="n">
         <v>0.523</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="5" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -1019,7 +1045,7 @@
       <c r="C3" s="9" t="n">
         <v>0.57</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="5" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -1041,7 +1067,7 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -2027,6 +2053,1135 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E41"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B2" s="5" t="n">
+        <v>104.2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>122.4</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>140.6</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>158.8</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="n">
+        <v>2025</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>177</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="n">
+        <v>2026</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>195.2</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="n">
+        <v>2027</v>
+      </c>
+      <c r="B8" s="5" t="n">
+        <v>213.4</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E8" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="n">
+        <v>2028</v>
+      </c>
+      <c r="B9" s="5" t="n">
+        <v>231.6</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E9" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="n">
+        <v>2029</v>
+      </c>
+      <c r="B10" s="5" t="n">
+        <v>249.8</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="n">
+        <v>2030</v>
+      </c>
+      <c r="B11" s="5" t="n">
+        <v>268</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E11" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="n">
+        <v>2031</v>
+      </c>
+      <c r="B12" s="5" t="n">
+        <v>298</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E12" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="n">
+        <v>2032</v>
+      </c>
+      <c r="B13" s="5" t="n">
+        <v>328</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="n">
+        <v>2033</v>
+      </c>
+      <c r="B14" s="5" t="n">
+        <v>358</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="n">
+        <v>2034</v>
+      </c>
+      <c r="B15" s="5" t="n">
+        <v>388</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="n">
+        <v>2035</v>
+      </c>
+      <c r="B16" s="5" t="n">
+        <v>418</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E16" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="n">
+        <v>2036</v>
+      </c>
+      <c r="B17" s="5" t="n">
+        <v>447</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="n">
+        <v>2037</v>
+      </c>
+      <c r="B18" s="5" t="n">
+        <v>476</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E18" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="n">
+        <v>2038</v>
+      </c>
+      <c r="B19" s="5" t="n">
+        <v>505</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E19" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="n">
+        <v>2039</v>
+      </c>
+      <c r="B20" s="5" t="n">
+        <v>534</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E20" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="n">
+        <v>2040</v>
+      </c>
+      <c r="B21" s="5" t="n">
+        <v>563</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E21" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="n">
+        <v>2041</v>
+      </c>
+      <c r="B22" s="5" t="n">
+        <v>592</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="n">
+        <v>2042</v>
+      </c>
+      <c r="B23" s="5" t="n">
+        <v>621</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="n">
+        <v>2043</v>
+      </c>
+      <c r="B24" s="5" t="n">
+        <v>650</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E24" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5" t="n">
+        <v>2044</v>
+      </c>
+      <c r="B25" s="5" t="n">
+        <v>679</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E25" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="n">
+        <v>2045</v>
+      </c>
+      <c r="B26" s="5" t="n">
+        <v>708</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E26" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="n">
+        <v>2046</v>
+      </c>
+      <c r="B27" s="5" t="n">
+        <v>738</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E27" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="n">
+        <v>2047</v>
+      </c>
+      <c r="B28" s="5" t="n">
+        <v>768</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E28" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5" t="n">
+        <v>2048</v>
+      </c>
+      <c r="B29" s="5" t="n">
+        <v>798</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E29" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5" t="n">
+        <v>2049</v>
+      </c>
+      <c r="B30" s="5" t="n">
+        <v>828</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E30" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="n">
+        <v>2050</v>
+      </c>
+      <c r="B31" s="5" t="n">
+        <v>858</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E31" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="n">
+        <v>2051</v>
+      </c>
+      <c r="B32" s="5" t="n">
+        <v>858</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E32" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="5" t="n">
+        <v>2052</v>
+      </c>
+      <c r="B33" s="5" t="n">
+        <v>858</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D33" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E33" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="5" t="n">
+        <v>2053</v>
+      </c>
+      <c r="B34" s="5" t="n">
+        <v>858</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E34" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="5" t="n">
+        <v>2054</v>
+      </c>
+      <c r="B35" s="5" t="n">
+        <v>858</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D35" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E35" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="5" t="n">
+        <v>2055</v>
+      </c>
+      <c r="B36" s="5" t="n">
+        <v>858</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D36" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E36" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="5" t="n">
+        <v>2056</v>
+      </c>
+      <c r="B37" s="5" t="n">
+        <v>858</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D37" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E37" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="5" t="n">
+        <v>2057</v>
+      </c>
+      <c r="B38" s="5" t="n">
+        <v>858</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D38" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E38" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="5" t="n">
+        <v>2058</v>
+      </c>
+      <c r="B39" s="5" t="n">
+        <v>858</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D39" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E39" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="5" t="n">
+        <v>2059</v>
+      </c>
+      <c r="B40" s="5" t="n">
+        <v>858</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E40" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="5" t="n">
+        <v>2060</v>
+      </c>
+      <c r="B41" s="5" t="n">
+        <v>858</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D41" s="5" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E41" s="5" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="11.19"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>3180</v>
+      </c>
+      <c r="F2" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>0.206</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>3140</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>0.087</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" s="5" t="n">
+        <v>3140</v>
+      </c>
+      <c r="F8" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" s="5" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="F9" s="5" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <v>0.056</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E11" s="5" t="n">
+        <v>3140</v>
+      </c>
+      <c r="F11" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="5" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="F12" s="5" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>0.051</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>3140</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="5" t="n">
+        <v>0.051</v>
+      </c>
+      <c r="F16" s="5" t="n">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <v>3140</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" s="5" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="F18" s="5" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="5" t="n">
+        <v>0.051</v>
+      </c>
+      <c r="F19" s="5" t="n">
+        <v>298</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -2762,7 +3917,7 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -2905,8 +4060,8 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2999,7 +4154,7 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -3142,7 +4297,7 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix error in tunnel operation unit cost (inconsistency between Tab 5 and Tab 4 of Guidebook).
</commit_message>
<xml_diff>
--- a/pycba/parameters/svk/transport/OPIIv3p0/svk_road_cba_parameters_OPIIv3p0_2022.xlsx
+++ b/pycba/parameters/svk/transport/OPIIv3p0/svk_road_cba_parameters_OPIIv3p0_2022.xlsx
@@ -5618,7 +5618,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5804,7 +5804,8 @@
       <c r="C8" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="6" t="b">
+      <c r="D8" s="6" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="E8" s="5" t="n">
@@ -5827,7 +5828,8 @@
       <c r="C9" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="6" t="b">
+      <c r="D9" s="6" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="E9" s="5" t="n">
@@ -6042,7 +6044,8 @@
       <c r="C18" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="6" t="b">
+      <c r="D18" s="6" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="E18" s="5" t="n">
@@ -6065,7 +6068,8 @@
       <c r="C19" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="6" t="b">
+      <c r="D19" s="6" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="E19" s="5" t="n">
@@ -6147,7 +6151,8 @@
         <v>39</v>
       </c>
       <c r="G22" s="5" t="n">
-        <v>35</v>
+        <f aca="false">35+55</f>
+        <v>90</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6171,7 +6176,8 @@
         <v>39</v>
       </c>
       <c r="G23" s="5" t="n">
-        <v>28.5</v>
+        <f aca="false">28.5+55</f>
+        <v>83.5</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6195,7 +6201,8 @@
         <v>39</v>
       </c>
       <c r="G24" s="5" t="n">
-        <v>35</v>
+        <f aca="false">35+55</f>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix typo in CAPEX item name.
</commit_message>
<xml_diff>
--- a/pycba/parameters/svk/transport/OPIIv3p0/svk_road_cba_parameters_OPIIv3p0_2022.xlsx
+++ b/pycba/parameters/svk/transport/OPIIv3p0/svk_road_cba_parameters_OPIIv3p0_2022.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="residual_value" sheetId="1" state="visible" r:id="rId2"/>
@@ -114,7 +114,7 @@
     <t xml:space="preserve">induced investment</t>
   </si>
   <si>
-    <t xml:space="preserve">supervison</t>
+    <t xml:space="preserve">supervision</t>
   </si>
   <si>
     <t xml:space="preserve">other services</t>
@@ -606,8 +606,8 @@
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5617,7 +5617,7 @@
   </sheetPr>
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
     </sheetView>
   </sheetViews>

</xml_diff>